<commit_message>
add Jang's framework validation
</commit_message>
<xml_diff>
--- a/lambda_n_lt1.xlsx
+++ b/lambda_n_lt1.xlsx
@@ -84,7 +84,7 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>0.61920262254109026</v>
+        <v>0.6192928068550323</v>
       </c>
       <c r="B2" s="0">
         <v>0.10000000000000001</v>
@@ -92,7 +92,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>0.62021590627274803</v>
+        <v>0.6203056233230444</v>
       </c>
       <c r="B3" s="0">
         <v>0.11</v>
@@ -100,7 +100,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>0.62120016866513161</v>
+        <v>0.62128942958425271</v>
       </c>
       <c r="B4" s="0">
         <v>0.12000000000000001</v>
@@ -108,7 +108,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>0.62215653655763559</v>
+        <v>0.62224535220941535</v>
       </c>
       <c r="B5" s="0">
         <v>0.13</v>
@@ -116,7 +116,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>0.62308608525208176</v>
+        <v>0.62317446623017392</v>
       </c>
       <c r="B6" s="0">
         <v>0.14000000000000001</v>
@@ -124,7 +124,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>0.62398984137974334</v>
+        <v>0.62407779800728591</v>
       </c>
       <c r="B7" s="0">
         <v>0.15000000000000002</v>
@@ -132,7 +132,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>0.62486878537579915</v>
+        <v>0.62495632770623566</v>
       </c>
       <c r="B8" s="0">
         <v>0.16</v>
@@ -140,7 +140,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>0.62572385371746653</v>
+        <v>0.62581099153641129</v>
       </c>
       <c r="B9" s="0">
         <v>0.17000000000000001</v>
@@ -148,7 +148,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>0.62655594100558942</v>
+        <v>0.62664268383360133</v>
       </c>
       <c r="B10" s="0">
         <v>0.17999999999999999</v>
@@ -156,7 +156,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>0.62736590193108588</v>
+        <v>0.62745225902721347</v>
       </c>
       <c r="B11" s="0">
         <v>0.19</v>
@@ -164,7 +164,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>0.62815455314788993</v>
+        <v>0.62824053351385867</v>
       </c>
       <c r="B12" s="0">
         <v>0.20000000000000001</v>
@@ -172,7 +172,7 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>0.6289226750637853</v>
+        <v>0.6290082874487084</v>
       </c>
       <c r="B13" s="0">
         <v>0.21000000000000002</v>
@@ -180,7 +180,7 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>0.62967101355522381</v>
+        <v>0.62975626646073146</v>
       </c>
       <c r="B14" s="0">
         <v>0.22</v>
@@ -188,7 +188,7 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>0.63040028160956174</v>
+        <v>0.63048518329525749</v>
       </c>
       <c r="B15" s="0">
         <v>0.23000000000000001</v>
@@ -196,7 +196,7 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>0.63111116089688379</v>
+        <v>0.63119571938604813</v>
       </c>
       <c r="B16" s="0">
         <v>0.24000000000000002</v>
@@ -204,7 +204,7 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>0.63180430327307158</v>
+        <v>0.63188852635854165</v>
       </c>
       <c r="B17" s="0">
         <v>0.25</v>
@@ -212,7 +212,7 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>0.63248033221563593</v>
+        <v>0.63256422746580609</v>
       </c>
       <c r="B18" s="0">
         <v>0.26000000000000001</v>
@@ -220,7 +220,7 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>0.63313984419389269</v>
+        <v>0.63322341895878254</v>
       </c>
       <c r="B19" s="0">
         <v>0.27000000000000002</v>
@@ -228,7 +228,7 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>0.63378340997518245</v>
+        <v>0.63386667139253272</v>
       </c>
       <c r="B20" s="0">
         <v>0.28000000000000003</v>
@@ -236,7 +236,7 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>0.63441157586899222</v>
+        <v>0.6344945308703509</v>
       </c>
       <c r="B21" s="0">
         <v>0.29000000000000004</v>
@@ -244,7 +244,7 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>0.63502486491096544</v>
+        <v>0.63510752022773553</v>
       </c>
       <c r="B22" s="0">
         <v>0.30000000000000004</v>
@@ -252,7 +252,7 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>0.63562377798890424</v>
+        <v>0.63570614015832971</v>
       </c>
       <c r="B23" s="0">
         <v>0.31</v>
@@ -260,7 +260,7 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>0.6362087949129509</v>
+        <v>0.63629087028401832</v>
       </c>
       <c r="B24" s="0">
         <v>0.32000000000000001</v>
@@ -268,7 +268,7 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>0.63678037543218469</v>
+        <v>0.6368621701714261</v>
       </c>
       <c r="B25" s="0">
         <v>0.33000000000000002</v>
@@ -276,7 +276,7 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>0.63733896019989777</v>
+        <v>0.63742048029708154</v>
       </c>
       <c r="B26" s="0">
         <v>0.33999999999999997</v>
@@ -284,7 +284,7 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>0.63788497168981795</v>
+        <v>0.63796622296351602</v>
       </c>
       <c r="B27" s="0">
         <v>0.34999999999999998</v>
@@ -292,7 +292,7 @@
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>0.63841881506552001</v>
+        <v>0.63849980316854571</v>
       </c>
       <c r="B28" s="0">
         <v>0.35999999999999999</v>
@@ -300,7 +300,7 @@
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>0.63894087900524066</v>
+        <v>0.63902160942994868</v>
       </c>
       <c r="B29" s="0">
         <v>0.37</v>
@@ -308,7 +308,7 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>0.63945153648425368</v>
+        <v>0.63953201456770037</v>
       </c>
       <c r="B30" s="0">
         <v>0.38</v>
@@ -316,7 +316,7 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>0.63995114551691179</v>
+        <v>0.64003137644587194</v>
       </c>
       <c r="B31" s="0">
         <v>0.39000000000000001</v>
@@ -324,7 +324,7 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>0.64044004986038749</v>
+        <v>0.64052003867622553</v>
       </c>
       <c r="B32" s="0">
         <v>0.40000000000000002</v>
@@ -332,7 +332,7 @@
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>0.64091857968207622</v>
+        <v>0.64099833128547246</v>
       </c>
       <c r="B33" s="0">
         <v>0.41000000000000003</v>
@@ -340,7 +340,7 @@
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>0.64138705219254755</v>
+        <v>0.64146657134807927</v>
       </c>
       <c r="B34" s="0">
         <v>0.42000000000000004</v>
@@ -348,7 +348,7 @@
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>0.64184577224585282</v>
+        <v>0.64192506358643142</v>
       </c>
       <c r="B35" s="0">
         <v>0.43000000000000005</v>
@@ -356,7 +356,7 @@
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>0.64229503290891599</v>
+        <v>0.64237410094008174</v>
       </c>
       <c r="B36" s="0">
         <v>0.44000000000000006</v>
@@ -364,7 +364,7 @@
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>0.64273511600165767</v>
+        <v>0.6428139651057343</v>
       </c>
       <c r="B37" s="0">
         <v>0.45000000000000007</v>
@@ -372,7 +372,7 @@
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>0.64316629260942049</v>
+        <v>0.64324492704953218</v>
       </c>
       <c r="B38" s="0">
         <v>0.45999999999999996</v>
@@ -380,7 +380,7 @@
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>0.64358882356918945</v>
+        <v>0.64366724749314308</v>
       </c>
       <c r="B39" s="0">
         <v>0.46999999999999997</v>
@@ -388,7 +388,7 @@
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>0.64400295993102397</v>
+        <v>0.64408117737505988</v>
       </c>
       <c r="B40" s="0">
         <v>0.47999999999999998</v>
@@ -396,7 +396,7 @@
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>0.6444089433960456</v>
+        <v>0.64448695828845937</v>
       </c>
       <c r="B41" s="0">
         <v>0.48999999999999999</v>
@@ -404,7 +404,7 @@
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>0.64480700673225433</v>
+        <v>0.64488482289689397</v>
       </c>
       <c r="B42" s="0">
         <v>0.5</v>
@@ -412,7 +412,7 @@
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>0.64519737416937895</v>
+        <v>0.64527499532902055</v>
       </c>
       <c r="B43" s="0">
         <v>0.51000000000000001</v>
@@ -420,7 +420,7 @@
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>0.64558026177390149</v>
+        <v>0.64565769155350727</v>
       </c>
       <c r="B44" s="0">
         <v>0.52000000000000002</v>
@@ -428,7 +428,7 @@
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>0.64595587780533448</v>
+        <v>0.6460331197351955</v>
       </c>
       <c r="B45" s="0">
         <v>0.53000000000000003</v>
@@ -436,7 +436,7 @@
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>0.64632442305476689</v>
+        <v>0.64640148057353619</v>
       </c>
       <c r="B46" s="0">
         <v>0.54000000000000004</v>
@@ -444,7 +444,7 @@
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>0.64668609116664355</v>
+        <v>0.64676296762426166</v>
       </c>
       <c r="B47" s="0">
         <v>0.55000000000000004</v>
@@ -452,7 +452,7 @@
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>0.64704106894468427</v>
+        <v>0.64711776760520046</v>
       </c>
       <c r="B48" s="0">
         <v>0.56000000000000005</v>
@@ -460,7 +460,7 @@
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>0.64738953664280008</v>
+        <v>0.64746606068709467</v>
       </c>
       <c r="B49" s="0">
         <v>0.57000000000000006</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>0.64773166824181483</v>
+        <v>0.64780802077022415</v>
       </c>
       <c r="B50" s="0">
         <v>0.57999999999999996</v>
@@ -476,7 +476,7 @@
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>0.64806763171275694</v>
+        <v>0.64814381574760505</v>
       </c>
       <c r="B51" s="0">
         <v>0.58999999999999997</v>
@@ -484,7 +484,7 @@
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>0.64839758926743885</v>
+        <v>0.64847360775547924</v>
       </c>
       <c r="B52" s="0">
         <v>0.59999999999999998</v>
@@ -492,7 +492,7 @@
     </row>
     <row r="53">
       <c r="A53" s="0">
-        <v>0.64872169759700449</v>
+        <v>0.6487975534117757</v>
       </c>
       <c r="B53" s="0">
         <v>0.60999999999999999</v>
@@ -500,7 +500,7 @@
     </row>
     <row r="54">
       <c r="A54" s="0">
-        <v>0.64904010809908574</v>
+        <v>0.64911580404318225</v>
       </c>
       <c r="B54" s="0">
         <v>0.62</v>
@@ -508,7 +508,7 @@
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>0.64935296709416945</v>
+        <v>0.64942850590143308</v>
       </c>
       <c r="B55" s="0">
         <v>0.63</v>
@@ -516,7 +516,7 @@
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>0.64966041603174907</v>
+        <v>0.64973580036938172</v>
       </c>
       <c r="B56" s="0">
         <v>0.64000000000000001</v>
@@ -524,7 +524,7 @@
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>0.64996259168679338</v>
+        <v>0.65003782415739653</v>
       </c>
       <c r="B57" s="0">
         <v>0.65000000000000002</v>
@@ -532,7 +532,7 @@
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>0.65025962634704471</v>
+        <v>0.65033470949058503</v>
       </c>
       <c r="B58" s="0">
         <v>0.66000000000000003</v>
@@ -540,7 +540,7 @@
     </row>
     <row r="59">
       <c r="A59" s="0">
-        <v>0.65055164799162002</v>
+        <v>0.65062658428732778</v>
       </c>
       <c r="B59" s="0">
         <v>0.67000000000000004</v>
@@ -548,7 +548,7 @@
     </row>
     <row r="60">
       <c r="A60" s="0">
-        <v>0.65083878046137111</v>
+        <v>0.65091357232957059</v>
       </c>
       <c r="B60" s="0">
         <v>0.67999999999999994</v>
@@ -556,7 +556,7 @@
     </row>
     <row r="61">
       <c r="A61" s="0">
-        <v>0.65112114362142637</v>
+        <v>0.65119579342530198</v>
       </c>
       <c r="B61" s="0">
         <v>0.68999999999999995</v>
@@ -564,7 +564,7 @@
     </row>
     <row r="62">
       <c r="A62" s="0">
-        <v>0.65139885351631754</v>
+        <v>0.6514733635636194</v>
       </c>
       <c r="B62" s="0">
         <v>0.69999999999999996</v>
@@ -572,7 +572,7 @@
     </row>
     <row r="63">
       <c r="A63" s="0">
-        <v>0.65167202251807255</v>
+        <v>0.65174639506276166</v>
       </c>
       <c r="B63" s="0">
         <v>0.70999999999999996</v>
@@ -580,7 +580,7 @@
     </row>
     <row r="64">
       <c r="A64" s="0">
-        <v>0.65194075946763042</v>
+        <v>0.65201499671146712</v>
       </c>
       <c r="B64" s="0">
         <v>0.71999999999999997</v>
@@ -588,7 +588,7 @@
     </row>
     <row r="65">
       <c r="A65" s="0">
-        <v>0.65220516980991838</v>
+        <v>0.65227927390399587</v>
       </c>
       <c r="B65" s="0">
         <v>0.72999999999999998</v>
@@ -596,7 +596,7 @@
     </row>
     <row r="66">
       <c r="A66" s="0">
-        <v>0.65246535572291153</v>
+        <v>0.65253932876913623</v>
       </c>
       <c r="B66" s="0">
         <v>0.73999999999999999</v>
@@ -604,7 +604,7 @@
     </row>
     <row r="67">
       <c r="A67" s="0">
-        <v>0.65272141624097479</v>
+        <v>0.65279526029349577</v>
       </c>
       <c r="B67" s="0">
         <v>0.75</v>
@@ -612,7 +612,7 @@
     </row>
     <row r="68">
       <c r="A68" s="0">
-        <v>0.65297344737277585</v>
+        <v>0.65304716443936572</v>
       </c>
       <c r="B68" s="0">
         <v>0.76000000000000001</v>
@@ -620,7 +620,7 @@
     </row>
     <row r="69">
       <c r="A69" s="0">
-        <v>0.65322154221403561</v>
+        <v>0.65329513425742414</v>
       </c>
       <c r="B69" s="0">
         <v>0.77000000000000002</v>
@@ -628,7 +628,7 @@
     </row>
     <row r="70">
       <c r="A70" s="0">
-        <v>0.65346579105537472</v>
+        <v>0.65353925999453677</v>
       </c>
       <c r="B70" s="0">
         <v>0.78000000000000003</v>
@@ -636,7 +636,7 @@
     </row>
     <row r="71">
       <c r="A71" s="0">
-        <v>0.65370628148549459</v>
+        <v>0.6537796291968947</v>
       </c>
       <c r="B71" s="0">
         <v>0.79000000000000004</v>
@@ -644,7 +644,7 @@
     </row>
     <row r="72">
       <c r="A72" s="0">
-        <v>0.65394309848992271</v>
+        <v>0.65401632680871791</v>
       </c>
       <c r="B72" s="0">
         <v>0.80000000000000004</v>
@@ -652,7 +652,7 @@
     </row>
     <row r="73">
       <c r="A73" s="0">
-        <v>0.65417632454553709</v>
+        <v>0.65424943526673929</v>
       </c>
       <c r="B73" s="0">
         <v>0.80999999999999994</v>
@@ -660,7 +660,7 @@
     </row>
     <row r="74">
       <c r="A74" s="0">
-        <v>0.65440603971107603</v>
+        <v>0.65447903459067525</v>
       </c>
       <c r="B74" s="0">
         <v>0.81999999999999995</v>
@@ -668,7 +668,7 @@
     </row>
     <row r="75">
       <c r="A75" s="0">
-        <v>0.65463232171382413</v>
+        <v>0.6547052024698744</v>
       </c>
       <c r="B75" s="0">
         <v>0.82999999999999996</v>
@@ -676,7 +676,7 @@
     </row>
     <row r="76">
       <c r="A76" s="0">
-        <v>0.65485524603265932</v>
+        <v>0.65492801434632886</v>
       </c>
       <c r="B76" s="0">
         <v>0.83999999999999997</v>
@@ -684,7 +684,7 @@
     </row>
     <row r="77">
       <c r="A77" s="0">
-        <v>0.65507488597763397</v>
+        <v>0.65514754349422033</v>
       </c>
       <c r="B77" s="0">
         <v>0.84999999999999998</v>
@@ -692,7 +692,7 @@
     </row>
     <row r="78">
       <c r="A78" s="0">
-        <v>0.65529131276625374</v>
+        <v>0.65536386109616596</v>
       </c>
       <c r="B78" s="0">
         <v>0.85999999999999999</v>
@@ -700,7 +700,7 @@
     </row>
     <row r="79">
       <c r="A79" s="0">
-        <v>0.65550459559661123</v>
+        <v>0.65557703631631947</v>
       </c>
       <c r="B79" s="0">
         <v>0.87</v>
@@ -708,7 +708,7 @@
     </row>
     <row r="80">
       <c r="A80" s="0">
-        <v>0.65571480171751917</v>
+        <v>0.65578713637047403</v>
       </c>
       <c r="B80" s="0">
         <v>0.88</v>
@@ -716,7 +716,7 @@
     </row>
     <row r="81">
       <c r="A81" s="0">
-        <v>0.65592199649578786</v>
+        <v>0.65599422659330875</v>
       </c>
       <c r="B81" s="0">
         <v>0.89000000000000001</v>
@@ -724,7 +724,7 @@
     </row>
     <row r="82">
       <c r="A82" s="0">
-        <v>0.65612624348077253</v>
+        <v>0.65619837050290908</v>
       </c>
       <c r="B82" s="0">
         <v>0.90000000000000002</v>
@@ -732,7 +732,7 @@
     </row>
     <row r="83">
       <c r="A83" s="0">
-        <v>0.65632760446632399</v>
+        <v>0.65639962986268796</v>
       </c>
       <c r="B83" s="0">
         <v>0.91000000000000003</v>
@@ -740,7 +740,7 @@
     </row>
     <row r="84">
       <c r="A84" s="0">
-        <v>0.65652613955025529</v>
+        <v>0.65659806474082727</v>
       </c>
       <c r="B84" s="0">
         <v>0.92000000000000004</v>
@@ -748,7 +748,7 @@
     </row>
     <row r="85">
       <c r="A85" s="0">
-        <v>0.65672190719144241</v>
+        <v>0.65679373356735216</v>
       </c>
       <c r="B85" s="0">
         <v>0.93000000000000005</v>
@@ -756,7 +756,7 @@
     </row>
     <row r="86">
       <c r="A86" s="0">
-        <v>0.65691496426466345</v>
+        <v>0.65698669318894565</v>
       </c>
       <c r="B86" s="0">
         <v>0.93999999999999995</v>
@@ -764,7 +764,7 @@
     </row>
     <row r="87">
       <c r="A87" s="0">
-        <v>0.65710536611328041</v>
+        <v>0.65717699892160664</v>
       </c>
       <c r="B87" s="0">
         <v>0.94999999999999996</v>
@@ -772,7 +772,7 @@
     </row>
     <row r="88">
       <c r="A88" s="0">
-        <v>0.65729316659985815</v>
+        <v>0.65736470460124607</v>
       </c>
       <c r="B88" s="0">
         <v>0.95999999999999996</v>
@@ -780,7 +780,7 @@
     </row>
     <row r="89">
       <c r="A89" s="0">
-        <v>0.65747841815481589</v>
+        <v>0.65754986263231596</v>
       </c>
       <c r="B89" s="0">
         <v>0.96999999999999997</v>
@@ -788,7 +788,7 @@
     </row>
     <row r="90">
       <c r="A90" s="0">
-        <v>0.65766117182319539</v>
+        <v>0.65773252403455607</v>
       </c>
       <c r="B90" s="0">
         <v>0.97999999999999998</v>
@@ -796,7 +796,7 @@
     </row>
     <row r="91">
       <c r="A91" s="0">
-        <v>0.65784147730963061</v>
+        <v>0.65791273848794418</v>
       </c>
       <c r="B91" s="0">
         <v>0.98999999999999999</v>

</xml_diff>

<commit_message>
update for kenic geometry
</commit_message>
<xml_diff>
--- a/lambda_n_lt1.xlsx
+++ b/lambda_n_lt1.xlsx
@@ -84,7 +84,7 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>0.6192928068550323</v>
+        <v>0.56315883341524242</v>
       </c>
       <c r="B2" s="0">
         <v>0.10000000000000001</v>
@@ -92,7 +92,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>0.6203056233230444</v>
+        <v>0.56447796499544467</v>
       </c>
       <c r="B3" s="0">
         <v>0.11</v>
@@ -100,7 +100,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>0.62128942958425271</v>
+        <v>0.5657613997973141</v>
       </c>
       <c r="B4" s="0">
         <v>0.12000000000000001</v>
@@ -108,7 +108,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>0.62224535220941535</v>
+        <v>0.56701037894739581</v>
       </c>
       <c r="B5" s="0">
         <v>0.13</v>
@@ -116,7 +116,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>0.62317446623017392</v>
+        <v>0.5682260982607602</v>
       </c>
       <c r="B6" s="0">
         <v>0.14000000000000001</v>
@@ -124,7 +124,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>0.62407779800728591</v>
+        <v>0.56940970994965845</v>
       </c>
       <c r="B7" s="0">
         <v>0.15000000000000002</v>
@@ -132,7 +132,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>0.62495632770623566</v>
+        <v>0.5705623239776253</v>
       </c>
       <c r="B8" s="0">
         <v>0.16</v>
@@ -140,7 +140,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>0.62581099153641129</v>
+        <v>0.57168500926470667</v>
       </c>
       <c r="B9" s="0">
         <v>0.17000000000000001</v>
@@ -148,7 +148,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>0.62664268383360133</v>
+        <v>0.57277879484228877</v>
       </c>
       <c r="B10" s="0">
         <v>0.17999999999999999</v>
@@ -156,7 +156,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>0.62745225902721347</v>
+        <v>0.57384467100238046</v>
       </c>
       <c r="B11" s="0">
         <v>0.19</v>
@@ -164,7 +164,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>0.62824053351385867</v>
+        <v>0.57488359045896442</v>
       </c>
       <c r="B12" s="0">
         <v>0.20000000000000001</v>
@@ -172,7 +172,7 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>0.6290082874487084</v>
+        <v>0.57589646952526719</v>
       </c>
       <c r="B13" s="0">
         <v>0.21000000000000002</v>
@@ -180,7 +180,7 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>0.62975626646073146</v>
+        <v>0.57688418930409657</v>
       </c>
       <c r="B14" s="0">
         <v>0.22</v>
@@ -188,7 +188,7 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>0.63048518329525749</v>
+        <v>0.5778475968854232</v>
       </c>
       <c r="B15" s="0">
         <v>0.23000000000000001</v>
@@ -196,7 +196,7 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>0.63119571938604813</v>
+        <v>0.57878750654441502</v>
       </c>
       <c r="B16" s="0">
         <v>0.24000000000000002</v>
@@ -204,7 +204,7 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>0.63188852635854165</v>
+        <v>0.57970470093319038</v>
       </c>
       <c r="B17" s="0">
         <v>0.25</v>
@@ -212,7 +212,7 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>0.63256422746580609</v>
+        <v>0.58059993226013029</v>
       </c>
       <c r="B18" s="0">
         <v>0.26000000000000001</v>
@@ -220,7 +220,7 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>0.63322341895878254</v>
+        <v>0.58147392345138216</v>
       </c>
       <c r="B19" s="0">
         <v>0.27000000000000002</v>
@@ -228,7 +228,7 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>0.63386667139253272</v>
+        <v>0.5823273692900498</v>
       </c>
       <c r="B20" s="0">
         <v>0.28000000000000003</v>
@@ -236,7 +236,7 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>0.6344945308703509</v>
+        <v>0.58316093752939746</v>
       </c>
       <c r="B21" s="0">
         <v>0.29000000000000004</v>
@@ -244,7 +244,7 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>0.63510752022773553</v>
+        <v>0.58397526997717242</v>
       </c>
       <c r="B22" s="0">
         <v>0.30000000000000004</v>
@@ -252,7 +252,7 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>0.63570614015832971</v>
+        <v>0.58477098354883805</v>
       </c>
       <c r="B23" s="0">
         <v>0.31</v>
@@ -260,7 +260,7 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>0.63629087028401832</v>
+        <v>0.58554867128811794</v>
       </c>
       <c r="B24" s="0">
         <v>0.32000000000000001</v>
@@ -268,7 +268,7 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>0.6368621701714261</v>
+        <v>0.58630890335376518</v>
       </c>
       <c r="B25" s="0">
         <v>0.33000000000000002</v>
@@ -276,7 +276,7 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>0.63742048029708154</v>
+        <v>0.58705222797191314</v>
       </c>
       <c r="B26" s="0">
         <v>0.33999999999999997</v>
@@ -284,7 +284,7 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>0.63796622296351602</v>
+        <v>0.58777917235373067</v>
       </c>
       <c r="B27" s="0">
         <v>0.34999999999999998</v>
@@ -292,7 +292,7 @@
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>0.63849980316854571</v>
+        <v>0.58849024357841018</v>
       </c>
       <c r="B28" s="0">
         <v>0.35999999999999999</v>
@@ -300,7 +300,7 @@
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>0.63902160942994868</v>
+        <v>0.58918592944176662</v>
       </c>
       <c r="B29" s="0">
         <v>0.37</v>
@@ -308,7 +308,7 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>0.63953201456770037</v>
+        <v>0.58986669927092417</v>
       </c>
       <c r="B30" s="0">
         <v>0.38</v>
@@ -316,7 +316,7 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>0.64003137644587194</v>
+        <v>0.59053300470573467</v>
       </c>
       <c r="B31" s="0">
         <v>0.39000000000000001</v>
@@ -324,7 +324,7 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>0.64052003867622553</v>
+        <v>0.59118528044768903</v>
       </c>
       <c r="B32" s="0">
         <v>0.40000000000000002</v>
@@ -332,7 +332,7 @@
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>0.64099833128547246</v>
+        <v>0.59182394497719026</v>
       </c>
       <c r="B33" s="0">
         <v>0.41000000000000003</v>
@@ -340,7 +340,7 @@
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>0.64146657134807927</v>
+        <v>0.59244940124011836</v>
       </c>
       <c r="B34" s="0">
         <v>0.42000000000000004</v>
@@ -348,7 +348,7 @@
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>0.64192506358643142</v>
+        <v>0.59306203730467555</v>
       </c>
       <c r="B35" s="0">
         <v>0.43000000000000005</v>
@@ -356,7 +356,7 @@
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>0.64237410094008174</v>
+        <v>0.59366222698953175</v>
       </c>
       <c r="B36" s="0">
         <v>0.44000000000000006</v>
@@ -364,7 +364,7 @@
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>0.6428139651057343</v>
+        <v>0.59425033046430964</v>
       </c>
       <c r="B37" s="0">
         <v>0.45000000000000007</v>
@@ -372,7 +372,7 @@
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>0.64324492704953218</v>
+        <v>0.59482669482345807</v>
       </c>
       <c r="B38" s="0">
         <v>0.45999999999999996</v>
@@ -380,7 +380,7 @@
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>0.64366724749314308</v>
+        <v>0.5953916546345589</v>
       </c>
       <c r="B39" s="0">
         <v>0.46999999999999997</v>
@@ -388,7 +388,7 @@
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>0.64408117737505988</v>
+        <v>0.59594553246210413</v>
       </c>
       <c r="B40" s="0">
         <v>0.47999999999999998</v>
@@ -396,7 +396,7 @@
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>0.64448695828845937</v>
+        <v>0.59648863936776619</v>
       </c>
       <c r="B41" s="0">
         <v>0.48999999999999999</v>
@@ -404,7 +404,7 @@
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>0.64488482289689397</v>
+        <v>0.59702127538815919</v>
       </c>
       <c r="B42" s="0">
         <v>0.5</v>
@@ -412,7 +412,7 @@
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>0.64527499532902055</v>
+        <v>0.59754372999107064</v>
       </c>
       <c r="B43" s="0">
         <v>0.51000000000000001</v>
@@ -420,7 +420,7 @@
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>0.64565769155350727</v>
+        <v>0.59805628251110921</v>
       </c>
       <c r="B44" s="0">
         <v>0.52000000000000002</v>
@@ -428,7 +428,7 @@
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>0.6460331197351955</v>
+        <v>0.59855920256569228</v>
       </c>
       <c r="B45" s="0">
         <v>0.53000000000000003</v>
@@ -436,7 +436,7 @@
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>0.64640148057353619</v>
+        <v>0.59905275045225825</v>
       </c>
       <c r="B46" s="0">
         <v>0.54000000000000004</v>
@@ -444,7 +444,7 @@
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>0.64676296762426166</v>
+        <v>0.5995371775275643</v>
       </c>
       <c r="B47" s="0">
         <v>0.55000000000000004</v>
@@ -452,7 +452,7 @@
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>0.64711776760520046</v>
+        <v>0.60001272656989169</v>
       </c>
       <c r="B48" s="0">
         <v>0.56000000000000005</v>
@@ -460,7 +460,7 @@
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>0.64746606068709467</v>
+        <v>0.60047963212495248</v>
       </c>
       <c r="B49" s="0">
         <v>0.57000000000000006</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>0.64780802077022415</v>
+        <v>0.60093812083625853</v>
       </c>
       <c r="B50" s="0">
         <v>0.57999999999999996</v>
@@ -476,7 +476,7 @@
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>0.64814381574760505</v>
+        <v>0.60138841176067803</v>
       </c>
       <c r="B51" s="0">
         <v>0.58999999999999997</v>
@@ -484,7 +484,7 @@
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>0.64847360775547924</v>
+        <v>0.60183071666987975</v>
       </c>
       <c r="B52" s="0">
         <v>0.59999999999999998</v>
@@ -492,7 +492,7 @@
     </row>
     <row r="53">
       <c r="A53" s="0">
-        <v>0.6487975534117757</v>
+        <v>0.60226524033832829</v>
       </c>
       <c r="B53" s="0">
         <v>0.60999999999999999</v>
@@ -500,7 +500,7 @@
     </row>
     <row r="54">
       <c r="A54" s="0">
-        <v>0.64911580404318225</v>
+        <v>0.60269218081846831</v>
       </c>
       <c r="B54" s="0">
         <v>0.62</v>
@@ -508,7 +508,7 @@
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>0.64942850590143308</v>
+        <v>0.60311172970370186</v>
       </c>
       <c r="B55" s="0">
         <v>0.63</v>
@@ -516,7 +516,7 @@
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>0.64973580036938172</v>
+        <v>0.60352407237974237</v>
       </c>
       <c r="B56" s="0">
         <v>0.64000000000000001</v>
@@ -524,7 +524,7 @@
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>0.65003782415739653</v>
+        <v>0.60392938826489173</v>
       </c>
       <c r="B57" s="0">
         <v>0.65000000000000002</v>
@@ -532,7 +532,7 @@
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>0.65033470949058503</v>
+        <v>0.60432785103976949</v>
       </c>
       <c r="B58" s="0">
         <v>0.66000000000000003</v>
@@ -540,7 +540,7 @@
     </row>
     <row r="59">
       <c r="A59" s="0">
-        <v>0.65062658428732778</v>
+        <v>0.60471962886699382</v>
       </c>
       <c r="B59" s="0">
         <v>0.67000000000000004</v>
@@ -548,7 +548,7 @@
     </row>
     <row r="60">
       <c r="A60" s="0">
-        <v>0.65091357232957059</v>
+        <v>0.60510488460129019</v>
       </c>
       <c r="B60" s="0">
         <v>0.67999999999999994</v>
@@ -556,7 +556,7 @@
     </row>
     <row r="61">
       <c r="A61" s="0">
-        <v>0.65119579342530198</v>
+        <v>0.60548377599048187</v>
       </c>
       <c r="B61" s="0">
         <v>0.68999999999999995</v>
@@ -564,7 +564,7 @@
     </row>
     <row r="62">
       <c r="A62" s="0">
-        <v>0.6514733635636194</v>
+        <v>0.60585645586779246</v>
       </c>
       <c r="B62" s="0">
         <v>0.69999999999999996</v>
@@ -572,7 +572,7 @@
     </row>
     <row r="63">
       <c r="A63" s="0">
-        <v>0.65174639506276166</v>
+        <v>0.60622307233587269</v>
       </c>
       <c r="B63" s="0">
         <v>0.70999999999999996</v>
@@ -580,7 +580,7 @@
     </row>
     <row r="64">
       <c r="A64" s="0">
-        <v>0.65201499671146712</v>
+        <v>0.60658376894293942</v>
       </c>
       <c r="B64" s="0">
         <v>0.71999999999999997</v>
@@ -588,7 +588,7 @@
     </row>
     <row r="65">
       <c r="A65" s="0">
-        <v>0.65227927390399587</v>
+        <v>0.60693868485139868</v>
       </c>
       <c r="B65" s="0">
         <v>0.72999999999999998</v>
@@ -596,7 +596,7 @@
     </row>
     <row r="66">
       <c r="A66" s="0">
-        <v>0.65253932876913623</v>
+        <v>0.60728795499930621</v>
       </c>
       <c r="B66" s="0">
         <v>0.73999999999999999</v>
@@ -604,7 +604,7 @@
     </row>
     <row r="67">
       <c r="A67" s="0">
-        <v>0.65279526029349577</v>
+        <v>0.60763171025499962</v>
       </c>
       <c r="B67" s="0">
         <v>0.75</v>
@@ -612,7 +612,7 @@
     </row>
     <row r="68">
       <c r="A68" s="0">
-        <v>0.65304716443936572</v>
+        <v>0.60797007756522181</v>
       </c>
       <c r="B68" s="0">
         <v>0.76000000000000001</v>
@@ -620,7 +620,7 @@
     </row>
     <row r="69">
       <c r="A69" s="0">
-        <v>0.65329513425742414</v>
+        <v>0.60830318009703754</v>
       </c>
       <c r="B69" s="0">
         <v>0.77000000000000002</v>
@@ -628,7 +628,7 @@
     </row>
     <row r="70">
       <c r="A70" s="0">
-        <v>0.65353925999453677</v>
+        <v>0.60863113737383279</v>
       </c>
       <c r="B70" s="0">
         <v>0.78000000000000003</v>
@@ -636,7 +636,7 @@
     </row>
     <row r="71">
       <c r="A71" s="0">
-        <v>0.6537796291968947</v>
+        <v>0.60895406540566832</v>
       </c>
       <c r="B71" s="0">
         <v>0.79000000000000004</v>
@@ -644,7 +644,7 @@
     </row>
     <row r="72">
       <c r="A72" s="0">
-        <v>0.65401632680871791</v>
+        <v>0.60927207681425055</v>
       </c>
       <c r="B72" s="0">
         <v>0.80000000000000004</v>
@@ -652,7 +652,7 @@
     </row>
     <row r="73">
       <c r="A73" s="0">
-        <v>0.65424943526673929</v>
+        <v>0.60958528095276487</v>
       </c>
       <c r="B73" s="0">
         <v>0.80999999999999994</v>
@@ -660,7 +660,7 @@
     </row>
     <row r="74">
       <c r="A74" s="0">
-        <v>0.65447903459067525</v>
+        <v>0.60989378402080685</v>
       </c>
       <c r="B74" s="0">
         <v>0.81999999999999995</v>
@@ -668,7 +668,7 @@
     </row>
     <row r="75">
       <c r="A75" s="0">
-        <v>0.6547052024698744</v>
+        <v>0.61019768917463668</v>
       </c>
       <c r="B75" s="0">
         <v>0.82999999999999996</v>
@@ -676,7 +676,7 @@
     </row>
     <row r="76">
       <c r="A76" s="0">
-        <v>0.65492801434632886</v>
+        <v>0.61049709663296714</v>
       </c>
       <c r="B76" s="0">
         <v>0.83999999999999997</v>
@@ -684,7 +684,7 @@
     </row>
     <row r="77">
       <c r="A77" s="0">
-        <v>0.65514754349422033</v>
+        <v>0.61079210377848903</v>
       </c>
       <c r="B77" s="0">
         <v>0.84999999999999998</v>
@@ -692,7 +692,7 @@
     </row>
     <row r="78">
       <c r="A78" s="0">
-        <v>0.65536386109616596</v>
+        <v>0.6110828052553251</v>
       </c>
       <c r="B78" s="0">
         <v>0.85999999999999999</v>
@@ -700,7 +700,7 @@
     </row>
     <row r="79">
       <c r="A79" s="0">
-        <v>0.65557703631631947</v>
+        <v>0.61136929306259646</v>
       </c>
       <c r="B79" s="0">
         <v>0.87</v>
@@ -708,7 +708,7 @@
     </row>
     <row r="80">
       <c r="A80" s="0">
-        <v>0.65578713637047403</v>
+        <v>0.61165165664427501</v>
       </c>
       <c r="B80" s="0">
         <v>0.88</v>
@@ -716,7 +716,7 @@
     </row>
     <row r="81">
       <c r="A81" s="0">
-        <v>0.65599422659330875</v>
+        <v>0.61192998297548595</v>
       </c>
       <c r="B81" s="0">
         <v>0.89000000000000001</v>
@@ -724,7 +724,7 @@
     </row>
     <row r="82">
       <c r="A82" s="0">
-        <v>0.65619837050290908</v>
+        <v>0.6122043566454215</v>
       </c>
       <c r="B82" s="0">
         <v>0.90000000000000002</v>
@@ -732,7 +732,7 @@
     </row>
     <row r="83">
       <c r="A83" s="0">
-        <v>0.65639962986268796</v>
+        <v>0.61247485993701067</v>
       </c>
       <c r="B83" s="0">
         <v>0.91000000000000003</v>
@@ -740,7 +740,7 @@
     </row>
     <row r="84">
       <c r="A84" s="0">
-        <v>0.65659806474082727</v>
+        <v>0.61274157290349263</v>
       </c>
       <c r="B84" s="0">
         <v>0.92000000000000004</v>
@@ -748,7 +748,7 @@
     </row>
     <row r="85">
       <c r="A85" s="0">
-        <v>0.65679373356735216</v>
+        <v>0.61300457344202564</v>
       </c>
       <c r="B85" s="0">
         <v>0.93000000000000005</v>
@@ -756,7 +756,7 @@
     </row>
     <row r="86">
       <c r="A86" s="0">
-        <v>0.65698669318894565</v>
+        <v>0.61326393736446327</v>
       </c>
       <c r="B86" s="0">
         <v>0.93999999999999995</v>
@@ -764,7 +764,7 @@
     </row>
     <row r="87">
       <c r="A87" s="0">
-        <v>0.65717699892160664</v>
+        <v>0.6135197384654193</v>
       </c>
       <c r="B87" s="0">
         <v>0.94999999999999996</v>
@@ -772,7 +772,7 @@
     </row>
     <row r="88">
       <c r="A88" s="0">
-        <v>0.65736470460124607</v>
+        <v>0.61377204858774015</v>
       </c>
       <c r="B88" s="0">
         <v>0.95999999999999996</v>
@@ -780,7 +780,7 @@
     </row>
     <row r="89">
       <c r="A89" s="0">
-        <v>0.65754986263231596</v>
+        <v>0.61402093768549415</v>
       </c>
       <c r="B89" s="0">
         <v>0.96999999999999997</v>
@@ -788,7 +788,7 @@
     </row>
     <row r="90">
       <c r="A90" s="0">
-        <v>0.65773252403455607</v>
+        <v>0.61426647388458755</v>
       </c>
       <c r="B90" s="0">
         <v>0.97999999999999998</v>
@@ -796,7 +796,7 @@
     </row>
     <row r="91">
       <c r="A91" s="0">
-        <v>0.65791273848794418</v>
+        <v>0.61450872354110408</v>
       </c>
       <c r="B91" s="0">
         <v>0.98999999999999999</v>

</xml_diff>